<commit_message>
Solution for the second task is added
</commit_message>
<xml_diff>
--- a/DynamoDBSQL/dynamosql/src/assets/csv/one-to-many.xlsx
+++ b/DynamoDBSQL/dynamosql/src/assets/csv/one-to-many.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490"/>
   </bookViews>
   <sheets>
     <sheet name="orgs" sheetId="1" r:id="rId1"/>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,9 +477,9 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A21" si="0">A3+1</f>
+        <f t="shared" ref="A4" si="0">A3+1</f>
         <v>321543</v>
       </c>
       <c r="B4" t="s">
@@ -489,57 +489,6 @@
         <v>1968</v>
       </c>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -551,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +554,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A12" si="0">A3+1</f>
+        <f t="shared" ref="A4:A5" si="0">A3+1</f>
         <v>62373</v>
       </c>
       <c r="B4" t="s">

</xml_diff>